<commit_message>
Resolved issues #23, #34 and #47 and documented the flow profile specifications in a new documentation file outputProfileSpecification.md. Also restructuring and tidying up of venco_main.py
</commit_message>
<xml_diff>
--- a/inputData/VencoPy_scalarInput.xlsx
+++ b/inputData/VencoPy_scalarInput.xlsx
@@ -195,10 +195,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -504,7 +504,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -540,10 +540,10 @@
       <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="18"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -558,7 +558,7 @@
       <c r="N5" s="15"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -582,7 +582,7 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Some setup and installation ammendments, minor file cleanups
</commit_message>
<xml_diff>
--- a/inputData/VencoPy_scalarInput.xlsx
+++ b/inputData/VencoPy_scalarInput.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20367"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vencopy_repo\inputData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E68BD03-E3B1-4FD3-8D8A-8FD490D2D35E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="420" windowWidth="28515" windowHeight="12285"/>
+    <workbookView xWindow="120" yWindow="420" windowWidth="28515" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs of Model" sheetId="1" r:id="rId1"/>
@@ -103,7 +109,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -210,14 +216,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -255,9 +264,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -290,9 +299,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -325,9 +351,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -500,11 +543,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>